<commit_message>
[MIG] 12.0 account_bank_statement_import_adyen, account_bank_statement_clearing_account
</commit_message>
<xml_diff>
--- a/account_bank_statement_import_adyen/test_files/adyen_test.xlsx
+++ b/account_bank_statement_import_adyen/test_files/adyen_test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="995" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -127,7 +127,7 @@
     <t xml:space="preserve">Settled</t>
   </si>
   <si>
-    <t xml:space="preserve">EUR</t>
+    <t xml:space="preserve">USD</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;auto&gt;</t>
@@ -155,13 +155,14 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0.00"/>
-    <numFmt numFmtId="166" formatCode="YYYY\-MM\-DD\ HH:MM:SS"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -286,12 +287,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -301,7 +302,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>25920</xdr:colOff>
+      <xdr:colOff>26280</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>93240</xdr:rowOff>
     </xdr:from>
@@ -309,7 +310,7 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>180000</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>68040</xdr:rowOff>
+      <xdr:rowOff>67680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -322,8 +323,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="838440" y="93240"/>
-          <a:ext cx="3593880" cy="462240"/>
+          <a:off x="838800" y="93240"/>
+          <a:ext cx="3593520" cy="461880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -345,24 +346,21 @@
   </sheetPr>
   <dimension ref="B1:AE25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V5" activeCellId="0" sqref="V5:V23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L9" activeCellId="0" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.2295918367347"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.3622448979592"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.7040816326531"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.8877551020408"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.1173469387755"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="42.9285714285714"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.6122448979592"/>
-    <col collapsed="false" hidden="false" max="21" min="11" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="25.1428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="37.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="26.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="42.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="23.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="17.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="25.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -843,7 +841,7 @@
       </c>
       <c r="L10" s="5"/>
       <c r="M10" s="5" t="n">
-        <v>666</v>
+        <v>1598</v>
       </c>
       <c r="N10" s="5" t="n">
         <v>1</v>
@@ -1909,7 +1907,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>